<commit_message>
Cambio para el print del excel
</commit_message>
<xml_diff>
--- a/src/edu_pad/static/xlsx/Productos_Panamericana.xlsx
+++ b/src/edu_pad/static/xlsx/Productos_Panamericana.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,16 @@
           <t>URL</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Busqueda</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-05-22 04:14</t>
+          <t>2025-05-22 17:56</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -474,13 +479,18 @@
       <c r="D2" t="inlineStr">
         <is>
           <t>https://www.panamericana.com.co/percy-j-dioses-del-olimpo-1-ladron-del-rayo-612866/p</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>percy</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-05-22 04:14</t>
+          <t>2025-05-22 17:56</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -496,13 +506,18 @@
       <c r="D3" t="inlineStr">
         <is>
           <t>https://www.panamericana.com.co/percy-jackson-and-the-olympians-5-books-box-680026/p</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>percy</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-05-22 04:14</t>
+          <t>2025-05-22 17:56</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -518,13 +533,18 @@
       <c r="D4" t="inlineStr">
         <is>
           <t>https://www.panamericana.com.co/percy-j-dioses-del-olimpo-3-maldicion-del-titan-614101/p</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>percy</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-05-22 04:14</t>
+          <t>2025-05-22 17:56</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -540,13 +560,18 @@
       <c r="D5" t="inlineStr">
         <is>
           <t>https://www.panamericana.com.co/percy-jackson-y-los-dioses-del-olimpo-la-diosa-de-tres-cabezas-688733/p</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>percy</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-05-22 04:14</t>
+          <t>2025-05-22 17:56</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -562,13 +587,18 @@
       <c r="D6" t="inlineStr">
         <is>
           <t>https://www.panamericana.com.co/percy-jackson-and-the-olympians-the-battle-of-the-labyrinth-573456/p</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>percy</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-05-22 04:14</t>
+          <t>2025-05-22 17:56</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -584,13 +614,18 @@
       <c r="D7" t="inlineStr">
         <is>
           <t>https://www.panamericana.com.co/percy-j-dioses-del-olimpo-2-mar-de-los-monstruos-609423/p</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>percy</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-05-22 04:14</t>
+          <t>2025-05-22 17:56</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -606,13 +641,18 @@
       <c r="D8" t="inlineStr">
         <is>
           <t>https://www.panamericana.com.co/percy-jackson-y-los-dioses-del-olimpo-6-el-caliz-de-los-dioses-664626/p</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>percy</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-05-22 04:14</t>
+          <t>2025-05-22 17:56</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -628,13 +668,18 @@
       <c r="D9" t="inlineStr">
         <is>
           <t>https://www.panamericana.com.co/percy-jackson-and-the-olympians-1-thelightning-thief-368198/p</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>percy</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-05-22 04:14</t>
+          <t>2025-05-22 17:56</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -650,13 +695,18 @@
       <c r="D10" t="inlineStr">
         <is>
           <t>https://www.panamericana.com.co/percy-jackson-and-the-titans-curse/p</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>percy</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-05-22 04:14</t>
+          <t>2025-05-22 17:56</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -672,6 +722,11 @@
       <c r="D11" t="inlineStr">
         <is>
           <t>https://www.panamericana.com.co/la-ultima-descendiente-640440/p</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>percy</t>
         </is>
       </c>
     </row>

</xml_diff>